<commit_message>
Added function to pass keySequence
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
     <sheet name="testdata" sheetId="3" r:id="rId2"/>
+    <sheet name="system" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>username</t>
   </si>
@@ -123,6 +124,12 @@
   </si>
   <si>
     <t>testing123</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>systeem</t>
   </si>
 </sst>
 </file>
@@ -491,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,4 +789,68 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding HUB test case for Language check
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>username</t>
   </si>
@@ -123,13 +123,19 @@
     <t>objectID</t>
   </si>
   <si>
-    <t>testing123</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
     <t>systeem</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>hight</t>
+  </si>
+  <si>
+    <t>70px</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,15 +516,15 @@
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="12" width="26.85546875" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="7" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="14" width="26.85546875" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -541,25 +547,31 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -572,26 +584,26 @@
       <c r="G2">
         <v>560</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>365</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>370</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -604,26 +616,26 @@
       <c r="G3">
         <v>560</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>365</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>370</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>16</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>31</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -636,32 +648,29 @@
       <c r="G4">
         <v>560</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>365</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>370</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
@@ -677,32 +686,32 @@
       <c r="G5">
         <v>560</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5">
         <v>365</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>370</v>
       </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>19</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>31</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
@@ -718,26 +727,29 @@
       <c r="G6">
         <v>560</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6">
         <v>365</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>370</v>
       </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>19</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>31</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -795,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -844,10 +856,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new test case for Font check
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -132,10 +132,10 @@
     <t>width</t>
   </si>
   <si>
-    <t>hight</t>
-  </si>
-  <si>
     <t>70px</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
         <v>37</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>14</v>
@@ -687,10 +687,10 @@
         <v>560</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <v>365</v>
@@ -728,10 +728,10 @@
         <v>560</v>
       </c>
       <c r="H6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6">
         <v>365</v>

</xml_diff>

<commit_message>
Adding test cases for HUB left & right  navigation
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>username</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>HubMenu</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,9 +753,18 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
+      <c r="J7">
+        <v>365</v>
+      </c>
+      <c r="K7">
+        <v>370</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adding new Test Case files for Settings test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -4,25 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
-    <sheet name="testdata" sheetId="3" r:id="rId2"/>
-    <sheet name="system" sheetId="4" r:id="rId3"/>
+    <sheet name="screenTitles" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -114,18 +107,9 @@
     <t>"Proximus Light", ProximusLight</t>
   </si>
   <si>
-    <t>nitin</t>
-  </si>
-  <si>
-    <t>kaushik</t>
-  </si>
-  <si>
     <t>objectID</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>systeem</t>
   </si>
   <si>
@@ -139,6 +123,21 @@
   </si>
   <si>
     <t>HubMenu</t>
+  </si>
+  <si>
+    <t>epg</t>
+  </si>
+  <si>
+    <t>instellingen</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>epgSetting</t>
   </si>
 </sst>
 </file>
@@ -507,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,57 +528,57 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>85</v>
@@ -594,24 +593,24 @@
         <v>370</v>
       </c>
       <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" t="s">
         <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>365</v>
@@ -626,24 +625,24 @@
         <v>370</v>
       </c>
       <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
         <v>16</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4">
         <v>531</v>
@@ -658,30 +657,30 @@
         <v>370</v>
       </c>
       <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" t="s">
         <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="F5">
         <v>639</v>
@@ -690,10 +689,10 @@
         <v>560</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J5">
         <v>365</v>
@@ -702,27 +701,27 @@
         <v>370</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F6">
         <v>729</v>
@@ -731,10 +730,10 @@
         <v>560</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J6">
         <v>365</v>
@@ -743,18 +742,18 @@
         <v>370</v>
       </c>
       <c r="M6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -778,99 +777,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>123</v>
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Create EPG Test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Code\HTMLSelenium\src\test\java\com\rsystems\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
-    <sheet name="screenTitles" sheetId="6" r:id="rId2"/>
+    <sheet name="EpgScreen" sheetId="7" r:id="rId2"/>
+    <sheet name="screenTitles" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -138,13 +144,61 @@
   </si>
   <si>
     <t>epgSetting</t>
+  </si>
+  <si>
+    <t>rgba(242, 249, 250, 1)</t>
+  </si>
+  <si>
+    <t>programTitle</t>
+  </si>
+  <si>
+    <t>Proximus, ProximusBold</t>
+  </si>
+  <si>
+    <t>24px</t>
+  </si>
+  <si>
+    <t>rgba(128, 128, 128, 1)</t>
+  </si>
+  <si>
+    <t>rgba(255, 255, 0, 1)</t>
+  </si>
+  <si>
+    <t>EpgChannelScreen</t>
+  </si>
+  <si>
+    <t>donderdag, 25 mei</t>
+  </si>
+  <si>
+    <t>font_size</t>
+  </si>
+  <si>
+    <t>font_family</t>
+  </si>
+  <si>
+    <t>No_of_Channel</t>
+  </si>
+  <si>
+    <t>Seniour_groen_Grijs</t>
+  </si>
+  <si>
+    <t>Seniour_groen_Geel</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>20px</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -167,6 +221,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,12 +256,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -212,6 +273,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -260,7 +324,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,7 +359,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,7 +586,8 @@
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" customWidth="1"/>
     <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="14" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="30" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -777,15 +842,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M8" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -821,6 +1032,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Developed new testcases Releated to EPG SCreen
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -152,9 +152,6 @@
     <t>programTitle</t>
   </si>
   <si>
-    <t>Proximus, ProximusBold</t>
-  </si>
-  <si>
     <t>24px</t>
   </si>
   <si>
@@ -192,6 +189,39 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Seniour_Standard_Standard</t>
+  </si>
+  <si>
+    <t>Stark_Standard_Standard</t>
+  </si>
+  <si>
+    <t>Seniour_groen_Standard</t>
+  </si>
+  <si>
+    <t>Strak_groen_Standard</t>
+  </si>
+  <si>
+    <t>Strak_groen_grijs</t>
+  </si>
+  <si>
+    <t>Strak_groen_geel</t>
+  </si>
+  <si>
+    <t>Strak_Standard_grijs</t>
+  </si>
+  <si>
+    <t>Strak_Standard_geel</t>
+  </si>
+  <si>
+    <t>Seniour_Standard_geel</t>
+  </si>
+  <si>
+    <t>Seniour_Standard_grijs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programTitle </t>
   </si>
 </sst>
 </file>
@@ -842,10 +872,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,10 +930,10 @@
         <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>28</v>
@@ -912,18 +942,18 @@
         <v>15</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>17</v>
@@ -937,19 +967,19 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="L3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>45</v>
+      <c r="O3" t="s">
+        <v>16</v>
       </c>
       <c r="P3">
         <v>4</v>
@@ -957,27 +987,232 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>42</v>
       </c>
       <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O4" t="s">
-        <v>46</v>
       </c>
       <c r="P4">
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+    </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>43</v>
+      </c>
       <c r="M8" s="3" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="O8" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" t="s">
+        <v>16</v>
+      </c>
+      <c r="P10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" t="s">
+        <v>44</v>
+      </c>
+      <c r="P13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1034,10 +1269,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit rahul Tes cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14295" windowHeight="4230" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
     <sheet name="EpgScreen" sheetId="7" r:id="rId2"/>
-    <sheet name="screenTitles" sheetId="6" r:id="rId3"/>
+    <sheet name="library" sheetId="8" r:id="rId3"/>
+    <sheet name="screenTitles" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="86">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -222,6 +223,63 @@
   </si>
   <si>
     <t xml:space="preserve">programTitle </t>
+  </si>
+  <si>
+    <t>font-family</t>
+  </si>
+  <si>
+    <t>films, series en tv</t>
+  </si>
+  <si>
+    <t>32px</t>
+  </si>
+  <si>
+    <t>Proximus, "ProximusBold"</t>
+  </si>
+  <si>
+    <t>mijn apps</t>
+  </si>
+  <si>
+    <t>mijn planning</t>
+  </si>
+  <si>
+    <t>huidige gehuurde items</t>
+  </si>
+  <si>
+    <t>14px</t>
+  </si>
+  <si>
+    <t>Proximus, "ProximusRegular"</t>
+  </si>
+  <si>
+    <t>opnames</t>
+  </si>
+  <si>
+    <t>mijn Passen</t>
+  </si>
+  <si>
+    <t>herinneringen</t>
+  </si>
+  <si>
+    <t>geplande opnames</t>
+  </si>
+  <si>
+    <t>conflicten</t>
+  </si>
+  <si>
+    <t>Apps</t>
+  </si>
+  <si>
+    <t>pipSetting</t>
+  </si>
+  <si>
+    <t>pip</t>
+  </si>
+  <si>
+    <t>mijn bibliotheek</t>
+  </si>
+  <si>
+    <t>LiveTV</t>
   </si>
 </sst>
 </file>
@@ -874,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1223,10 +1281,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,6 +1510,30 @@
         <v>47</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create new test cases for EPG
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Code\HTMLSelenium\src\test\java\com\rsystems\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12705" windowHeight="3495" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12705" windowHeight="4515" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -12,14 +17,14 @@
     <sheet name="library" sheetId="8" r:id="rId3"/>
     <sheet name="screenTitles" sheetId="6" r:id="rId4"/>
     <sheet name="SystemInfoScreen" sheetId="9" r:id="rId5"/>
+    <sheet name="Films" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="103">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -313,6 +318,21 @@
   </si>
   <si>
     <t>systeeminfo</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>RentedMovieCategorie</t>
+  </si>
+  <si>
+    <t>RentedMovieName</t>
+  </si>
+  <si>
+    <t>AKGDCC1 NL Branch</t>
+  </si>
+  <si>
+    <t>AKG DCC VOD1</t>
   </si>
 </sst>
 </file>
@@ -1544,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1576,7 @@
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1564,7 +1584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1580,7 +1600,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -1588,7 +1608,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1596,7 +1616,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1604,7 +1624,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1612,7 +1632,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -1620,7 +1640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -1628,8 +1648,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1649,7 +1675,7 @@
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1657,7 +1683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -1665,7 +1691,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1673,7 +1699,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1681,12 +1707,55 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>95</v>
       </c>
       <c r="B5" s="5">
         <v>254479730</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit EPG and PIP Test cases for Release
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Code\HTMLSelenium\src\test\java\com\rsystems\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12705" windowHeight="4515" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="5085" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -19,13 +14,15 @@
     <sheet name="SystemInfoScreen" sheetId="9" r:id="rId5"/>
     <sheet name="Films" sheetId="10" r:id="rId6"/>
     <sheet name="parameters" sheetId="11" r:id="rId7"/>
+    <sheet name="PIPScreen" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:J14"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="136">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -403,6 +400,36 @@
   </si>
   <si>
     <t>language_FR</t>
+  </si>
+  <si>
+    <t>name_fr</t>
+  </si>
+  <si>
+    <t>paramètres</t>
+  </si>
+  <si>
+    <t>système</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>links</t>
+  </si>
+  <si>
+    <t>PIPLink</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>standaard</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>pip_position</t>
   </si>
 </sst>
 </file>
@@ -1643,51 +1670,64 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1695,7 +1735,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1703,7 +1743,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1711,7 +1751,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -1719,7 +1759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -1727,7 +1767,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -1735,7 +1775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>103</v>
       </c>
@@ -1743,7 +1783,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>105</v>
       </c>
@@ -1751,7 +1791,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>107</v>
       </c>
@@ -1985,4 +2025,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commit Few function uses in preetam test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Automation\HTML\HTMLSelenium\src\test\java\com\rsystems\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -15,14 +20,14 @@
     <sheet name="Films" sheetId="10" r:id="rId6"/>
     <sheet name="parameters" sheetId="11" r:id="rId7"/>
     <sheet name="PIPScreen" sheetId="12" r:id="rId8"/>
+    <sheet name="DTVChannel" sheetId="13" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:F12"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="145">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -430,6 +435,33 @@
   </si>
   <si>
     <t>language_NL</t>
+  </si>
+  <si>
+    <t>UnAvailiabeChannelNumber</t>
+  </si>
+  <si>
+    <t>ChannelNumber</t>
+  </si>
+  <si>
+    <t>ZapList</t>
+  </si>
+  <si>
+    <t>zaplijst</t>
+  </si>
+  <si>
+    <t>ExpectedFocousChannel</t>
+  </si>
+  <si>
+    <t>FirstChannelNumber</t>
+  </si>
+  <si>
+    <t>LastChannelNumber</t>
+  </si>
+  <si>
+    <t>HDChannelNumber</t>
+  </si>
+  <si>
+    <t>SDChannelNumber</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
@@ -1670,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,6 +1829,14 @@
       </c>
       <c r="B13" s="7" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1910,8 +1950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,10 +2072,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -2073,4 +2116,79 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Link selenium-stand-alone jar to POM.xml also add new jar guvva in dependenxy in pom.xml
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="149">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -440,9 +440,6 @@
     <t>UnAvailiabeChannelNumber</t>
   </si>
   <si>
-    <t>ChannelNumber</t>
-  </si>
-  <si>
     <t>ZapList</t>
   </si>
   <si>
@@ -462,6 +459,21 @@
   </si>
   <si>
     <t>SDChannelNumber</t>
+  </si>
+  <si>
+    <t>PauseButtonImagePath</t>
+  </si>
+  <si>
+    <t>PlayButtonImagePath</t>
+  </si>
+  <si>
+    <t>./resources/common/images/Pause_ON.png</t>
+  </si>
+  <si>
+    <t>./resources/common/images/Play_ON.png</t>
+  </si>
+  <si>
+    <t>Values</t>
   </si>
 </sst>
 </file>
@@ -1833,10 +1845,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2120,16 +2132,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2149,7 @@
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2150,7 +2162,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3">
         <v>323</v>
@@ -2158,7 +2170,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2166,7 +2178,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>999</v>
@@ -2174,7 +2186,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -2182,13 +2194,30 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit DTV Releated Test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="149">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -461,19 +461,19 @@
     <t>SDChannelNumber</t>
   </si>
   <si>
-    <t>PauseButtonImagePath</t>
-  </si>
-  <si>
-    <t>PlayButtonImagePath</t>
-  </si>
-  <si>
-    <t>./resources/common/images/Pause_ON.png</t>
-  </si>
-  <si>
-    <t>./resources/common/images/Play_ON.png</t>
-  </si>
-  <si>
     <t>Values</t>
+  </si>
+  <si>
+    <t>Pause_ON.png</t>
+  </si>
+  <si>
+    <t>Play_ON.png</t>
+  </si>
+  <si>
+    <t>PauseButtonImageName</t>
+  </si>
+  <si>
+    <t>PlayButtonImageName</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -564,6 +564,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2132,27 +2138,28 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -2160,7 +2167,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -2168,7 +2175,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -2176,7 +2183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -2184,7 +2191,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -2192,7 +2199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -2200,24 +2207,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B9" t="s">
-        <v>147</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" display="http://hpg.nat.myrio.net:8080/bepweb-1.0/resources/common/images/Play_ON.png"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rahul test case commited
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="parameters" sheetId="11" r:id="rId7"/>
     <sheet name="PIPScreen" sheetId="12" r:id="rId8"/>
     <sheet name="DTVChannel" sheetId="13" r:id="rId9"/>
+    <sheet name="MiniEPGScreen" sheetId="14" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="156">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -474,6 +475,27 @@
   </si>
   <si>
     <t>PlayButtonImageName</t>
+  </si>
+  <si>
+    <t>volgende</t>
+  </si>
+  <si>
+    <t>Future</t>
+  </si>
+  <si>
+    <t>bezig</t>
+  </si>
+  <si>
+    <t>InProgress</t>
+  </si>
+  <si>
+    <t>vorige</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>zoeken</t>
   </si>
 </sst>
 </file>
@@ -1147,6 +1169,53 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
@@ -1720,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,6 +1924,14 @@
       </c>
       <c r="B14" s="7" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2140,7 +2217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commit pritamm test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -22,13 +22,16 @@
     <sheet name="PIPScreen" sheetId="12" r:id="rId8"/>
     <sheet name="DTVChannel" sheetId="13" r:id="rId9"/>
     <sheet name="MiniEPGScreen" sheetId="14" r:id="rId10"/>
+    <sheet name="ActivateInfoBanner" sheetId="15" r:id="rId11"/>
+    <sheet name="TvFilterLayer" sheetId="16" r:id="rId12"/>
+    <sheet name="hotKeys" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="188">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -496,12 +499,111 @@
   </si>
   <si>
     <t>zoeken</t>
+  </si>
+  <si>
+    <t>http://poster.nat.myrio.net/default/t_0052_001.jpg</t>
+  </si>
+  <si>
+    <t>ChannelLogoFirst</t>
+  </si>
+  <si>
+    <t>RadioChannel</t>
+  </si>
+  <si>
+    <t>ChannelInfo</t>
+  </si>
+  <si>
+    <t>07:45 &gt; 08:25</t>
+  </si>
+  <si>
+    <t>ProgramDuration</t>
+  </si>
+  <si>
+    <t>Boucle de nuit</t>
+  </si>
+  <si>
+    <t>ProgramTitle</t>
+  </si>
+  <si>
+    <t>ChannelNo</t>
+  </si>
+  <si>
+    <t>VodHeading</t>
+  </si>
+  <si>
+    <t>VOD2 EN FR AUDIO SUB NL</t>
+  </si>
+  <si>
+    <t>Films</t>
+  </si>
+  <si>
+    <t>OnDemandMenu</t>
+  </si>
+  <si>
+    <t>op aanvraag</t>
+  </si>
+  <si>
+    <t>maa 19 jun</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>een tv-programma zoeken</t>
+  </si>
+  <si>
+    <t>radiozenders</t>
+  </si>
+  <si>
+    <t>RadioStations</t>
+  </si>
+  <si>
+    <t>voetbalkalender</t>
+  </si>
+  <si>
+    <t>FootballCalendar</t>
+  </si>
+  <si>
+    <t>voetbalzenders</t>
+  </si>
+  <si>
+    <t>FootballTV</t>
+  </si>
+  <si>
+    <t>nu op tv</t>
+  </si>
+  <si>
+    <t>Nowontv</t>
+  </si>
+  <si>
+    <t>nu</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>tv-gids</t>
+  </si>
+  <si>
+    <t>TvGrid</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>resources/components/animation/images/logo-white.png</t>
+  </si>
+  <si>
+    <t>Logo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,7 +675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -592,6 +694,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1173,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
@@ -1213,6 +1332,221 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="11">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1789,10 +2123,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,6 +2266,22 @@
       </c>
       <c r="B15" s="7" t="s">
         <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2000,16 +2350,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2034,6 +2384,14 @@
       </c>
       <c r="B3" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix priteam test cases bug
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="189">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -595,6 +595,9 @@
   </si>
   <si>
     <t>Logo</t>
+  </si>
+  <si>
+    <t>Heading</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1554,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,6 +1929,14 @@
       </c>
       <c r="Q14" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EPG font has been changed from 20 px to 21 px in Standard
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -195,9 +195,6 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>20px</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -598,6 +595,9 @@
   </si>
   <si>
     <t>Heading</t>
+  </si>
+  <si>
+    <t>21px</t>
   </si>
 </sst>
 </file>
@@ -1311,26 +1311,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1362,7 +1362,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="10">
         <v>2</v>
@@ -1370,23 +1370,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="11">
         <v>1</v>
@@ -1394,7 +1394,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="11">
         <v>800</v>
@@ -1402,10 +1402,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>10</v>
@@ -1449,50 +1449,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,15 +1500,15 @@
         <v>9</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +1558,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1629,7 @@
         <v>50</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1640,7 +1640,7 @@
         <v>42</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>54</v>
+        <v>188</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>17</v>
@@ -1652,15 +1652,15 @@
         <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
         <v>43</v>
@@ -1675,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="Q3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
         <v>4</v>
       </c>
       <c r="Q4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1721,12 +1721,12 @@
         <v>4</v>
       </c>
       <c r="Q5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
@@ -1744,12 +1744,12 @@
         <v>4</v>
       </c>
       <c r="Q6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
         <v>42</v>
@@ -1767,12 +1767,12 @@
         <v>4</v>
       </c>
       <c r="Q7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" t="s">
         <v>42</v>
@@ -1790,12 +1790,12 @@
         <v>4</v>
       </c>
       <c r="Q8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
@@ -1813,12 +1813,12 @@
         <v>6</v>
       </c>
       <c r="Q9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -1836,12 +1836,12 @@
         <v>6</v>
       </c>
       <c r="Q10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>42</v>
@@ -1859,12 +1859,12 @@
         <v>6</v>
       </c>
       <c r="Q11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
         <v>42</v>
@@ -1882,12 +1882,12 @@
         <v>6</v>
       </c>
       <c r="Q12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
@@ -1905,12 +1905,12 @@
         <v>6</v>
       </c>
       <c r="Q13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>42</v>
@@ -1928,12 +1928,12 @@
         <v>6</v>
       </c>
       <c r="Q14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
@@ -1941,12 +1941,12 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1981,7 +1981,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
         <v>15</v>
@@ -1989,142 +1989,142 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
         <v>69</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>74</v>
-      </c>
-      <c r="D5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
         <v>74</v>
-      </c>
-      <c r="D6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
         <v>74</v>
-      </c>
-      <c r="D7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" t="s">
         <v>74</v>
-      </c>
-      <c r="D8" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
         <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
         <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
         <v>74</v>
-      </c>
-      <c r="D11" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2155,7 +2155,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2166,7 +2166,7 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,10 +2201,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
         <v>82</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2212,12 +2212,12 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -2225,15 +2225,15 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
         <v>96</v>
-      </c>
-      <c r="B9" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2241,34 +2241,34 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2276,23 +2276,23 @@
         <v>9</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2324,31 +2324,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
         <v>91</v>
-      </c>
-      <c r="B3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="5">
         <v>254479730</v>
@@ -2383,26 +2383,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
         <v>165</v>
-      </c>
-      <c r="B4" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2435,82 +2435,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2552,29 +2552,29 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2602,12 +2602,12 @@
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>321</v>
@@ -2615,7 +2615,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3">
         <v>323</v>
@@ -2623,7 +2623,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2631,7 +2631,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5">
         <v>999</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -2655,21 +2655,21 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add sprint 3 test cases for Ankit
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="4320" firstSheet="11" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -25,13 +25,16 @@
     <sheet name="ActivateInfoBanner" sheetId="15" r:id="rId11"/>
     <sheet name="TvFilterLayer" sheetId="16" r:id="rId12"/>
     <sheet name="hotKeys" sheetId="17" r:id="rId13"/>
+    <sheet name="AccountInformation" sheetId="18" r:id="rId14"/>
+    <sheet name="ErrorMessages" sheetId="19" r:id="rId15"/>
+    <sheet name="RentMovie" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="203">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -598,6 +601,48 @@
   </si>
   <si>
     <t>21px</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>LineNumber</t>
+  </si>
+  <si>
+    <t>PinCode</t>
+  </si>
+  <si>
+    <t>0811</t>
+  </si>
+  <si>
+    <t>PLTV_Lock_Error_Message</t>
+  </si>
+  <si>
+    <t>Trickplay is not available, you are not subscribed to TSTV package, please contact Belgacom to subscribe</t>
+  </si>
+  <si>
+    <t>FOD</t>
+  </si>
+  <si>
+    <t>MovieName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preview KIDS </t>
+  </si>
+  <si>
+    <t>Carlitos droomt van voetbal (NL)</t>
+  </si>
+  <si>
+    <t>€0,00/24h</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -678,7 +723,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -714,6 +759,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1522,7 +1573,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,12 +1604,153 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,7 +2329,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit MiniEpg Regression test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Automation\HTML\HTMLSelenium\src\test\java\com\rsystems\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2910" firstSheet="11" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="4140" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -31,11 +26,12 @@
     <sheet name="Recording" sheetId="21" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:O12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="219">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -680,6 +676,18 @@
   </si>
   <si>
     <t>RecordingChannelNumber</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>gisteren</t>
+  </si>
+  <si>
+    <t>Tomorrow</t>
+  </si>
+  <si>
+    <t>morgen</t>
   </si>
 </sst>
 </file>
@@ -1117,24 +1125,24 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" customWidth="1"/>
     <col min="14" max="14" width="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="15" max="15" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1181,7 +1189,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1245,7 +1253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1318,7 +1326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1359,7 +1367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1385,18 +1393,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1404,7 +1412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -1412,7 +1420,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -1420,7 +1428,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1428,7 +1436,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -1436,12 +1444,28 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>213</v>
       </c>
       <c r="B6" s="17">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1457,13 +1481,13 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1471,7 +1495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>163</v>
       </c>
@@ -1479,7 +1503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>162</v>
       </c>
@@ -1487,7 +1511,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>160</v>
       </c>
@@ -1495,7 +1519,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>158</v>
       </c>
@@ -1503,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>157</v>
       </c>
@@ -1511,7 +1535,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>156</v>
       </c>
@@ -1536,13 +1560,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1550,7 +1574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>184</v>
       </c>
@@ -1558,7 +1582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>183</v>
       </c>
@@ -1566,7 +1590,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>181</v>
       </c>
@@ -1574,7 +1598,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>179</v>
       </c>
@@ -1582,7 +1606,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>177</v>
       </c>
@@ -1590,7 +1614,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>175</v>
       </c>
@@ -1598,7 +1622,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>173</v>
       </c>
@@ -1606,7 +1630,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1614,7 +1638,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>170</v>
       </c>
@@ -1636,13 +1660,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1650,7 +1674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -1672,13 +1696,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1686,7 +1710,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -1694,7 +1718,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -1702,7 +1726,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -1725,13 +1749,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1739,7 +1763,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -1760,15 +1784,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1785,7 +1809,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -1799,7 +1823,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -1826,17 +1850,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1844,7 +1868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>203</v>
       </c>
@@ -1852,7 +1876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>214</v>
       </c>
@@ -1873,25 +1897,25 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="12.140625" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="12.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="12.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.109375" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1944,7 +1968,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1967,7 +1991,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1990,7 +2014,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2013,7 +2037,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2036,7 +2060,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2059,7 +2083,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -2082,7 +2106,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2105,7 +2129,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2128,7 +2152,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -2151,7 +2175,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -2174,7 +2198,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -2197,7 +2221,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2220,7 +2244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2243,7 +2267,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -2251,12 +2275,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M18" s="3" t="s">
         <v>54</v>
       </c>
@@ -2275,14 +2299,14 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2299,7 +2323,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2313,7 +2337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2327,7 +2351,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -2341,7 +2365,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -2355,7 +2379,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -2369,7 +2393,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -2383,7 +2407,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -2397,7 +2421,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -2411,7 +2435,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -2425,7 +2449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -2452,14 +2476,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2470,7 +2494,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2481,7 +2505,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2492,7 +2516,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2503,7 +2527,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -2511,7 +2535,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -2519,7 +2543,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -2527,7 +2551,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -2535,7 +2559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2543,7 +2567,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -2551,7 +2575,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>102</v>
       </c>
@@ -2559,7 +2583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>104</v>
       </c>
@@ -2567,7 +2591,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>106</v>
       </c>
@@ -2575,7 +2599,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>136</v>
       </c>
@@ -2583,7 +2607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -2591,7 +2615,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>166</v>
       </c>
@@ -2599,7 +2623,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>167</v>
       </c>
@@ -2620,13 +2644,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -2634,7 +2658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -2642,7 +2666,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -2650,7 +2674,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -2658,7 +2682,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -2679,13 +2703,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2693,7 +2717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2701,7 +2725,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2709,7 +2733,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2717,7 +2741,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -2738,14 +2762,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2753,7 +2777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>123</v>
       </c>
@@ -2761,7 +2785,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>134</v>
       </c>
@@ -2769,7 +2793,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>120</v>
       </c>
@@ -2777,7 +2801,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>119</v>
       </c>
@@ -2785,7 +2809,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>117</v>
       </c>
@@ -2793,7 +2817,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>115</v>
       </c>
@@ -2801,7 +2825,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>113</v>
       </c>
@@ -2809,7 +2833,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>111</v>
       </c>
@@ -2817,7 +2841,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>110</v>
       </c>
@@ -2825,7 +2849,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>108</v>
       </c>
@@ -2833,15 +2857,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
@@ -2859,12 +2883,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2875,7 +2899,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -2886,7 +2910,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -2910,14 +2934,14 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2925,7 +2949,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -2933,7 +2957,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -2941,7 +2965,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -2949,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -2957,7 +2981,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -2965,7 +2989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -2973,7 +2997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -2984,7 +3008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -2992,7 +3016,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>210</v>
       </c>
@@ -3000,7 +3024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
Add  new film in test data and bug fix on old release
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="4140" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="3024" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -25,13 +25,13 @@
     <sheet name="RentMovie" sheetId="20" r:id="rId16"/>
     <sheet name="Recording" sheetId="21" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:O12"/>
+  <calcPr calcId="0" calcMode="manual"/>
+  <oleSize ref="A1:J8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="221">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t>morgen</t>
+  </si>
+  <si>
+    <t>POD1</t>
+  </si>
+  <si>
+    <t>Maya De Bij 3D</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1778,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1828,7 +1834,7 @@
         <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="C3" t="s">
         <v>209</v>
@@ -1840,6 +1846,24 @@
         <v>1111</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Developed BVT test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="3024" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="3024" firstSheet="14" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -29,13 +29,15 @@
     <sheet name="ErrorMessages" sheetId="19" r:id="rId15"/>
     <sheet name="RentMovie" sheetId="20" r:id="rId16"/>
     <sheet name="Recording" sheetId="21" r:id="rId17"/>
+    <sheet name="PackageAssignAndUnassign" sheetId="22" r:id="rId18"/>
+    <sheet name="MovieScreen" sheetId="23" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="269">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -725,6 +727,123 @@
   </si>
   <si>
     <t>CUTVEnabledChannelToPassForRecording_6</t>
+  </si>
+  <si>
+    <t>SubscriberAPIVersion</t>
+  </si>
+  <si>
+    <t>AccountNumber</t>
+  </si>
+  <si>
+    <t>PackageId</t>
+  </si>
+  <si>
+    <t>PackageLock</t>
+  </si>
+  <si>
+    <t>PackageUsoc</t>
+  </si>
+  <si>
+    <t>PackageRateCode</t>
+  </si>
+  <si>
+    <t>SubscriptionStartDate</t>
+  </si>
+  <si>
+    <t>SubcriptionEndDate</t>
+  </si>
+  <si>
+    <t>4.2.0</t>
+  </si>
+  <si>
+    <t>TVREPLAY</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>TVREPLAYF</t>
+  </si>
+  <si>
+    <t>70:TV-Replay</t>
+  </si>
+  <si>
+    <t>70:TV-Replay-Plus</t>
+  </si>
+  <si>
+    <t>POD2</t>
+  </si>
+  <si>
+    <t>POD3</t>
+  </si>
+  <si>
+    <t>POD4</t>
+  </si>
+  <si>
+    <t>Spiderman1</t>
+  </si>
+  <si>
+    <t>Spiderman2</t>
+  </si>
+  <si>
+    <t>Spiderman3</t>
+  </si>
+  <si>
+    <t>€0,00</t>
+  </si>
+  <si>
+    <t>€2,99</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Spiderman</t>
+  </si>
+  <si>
+    <t>GroupName</t>
+  </si>
+  <si>
+    <t>Assigned Package Id</t>
+  </si>
+  <si>
+    <t>First Movie Order</t>
+  </si>
+  <si>
+    <t>Benji</t>
+  </si>
+  <si>
+    <t>SortingOptionName</t>
+  </si>
+  <si>
+    <t>SortingOption1</t>
+  </si>
+  <si>
+    <t>SortingOption2</t>
+  </si>
+  <si>
+    <t>SortingOption3</t>
+  </si>
+  <si>
+    <t>SortingOption4</t>
+  </si>
+  <si>
+    <t>laatste kans</t>
+  </si>
+  <si>
+    <t>populair</t>
+  </si>
+  <si>
+    <t>a tot z</t>
+  </si>
+  <si>
+    <t>recent</t>
+  </si>
+  <si>
+    <t>25/07/2017</t>
+  </si>
+  <si>
+    <t>31/12/2020</t>
   </si>
 </sst>
 </file>
@@ -805,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -851,6 +970,24 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1159,7 +1296,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1815,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1827,9 +1964,11 @@
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1845,8 +1984,14 @@
       <c r="E1" s="2" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -1859,8 +2004,11 @@
       <c r="D2" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -1876,8 +2024,11 @@
       <c r="E3" s="17">
         <v>1111</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -1892,6 +2043,78 @@
       </c>
       <c r="E4" s="17">
         <v>1111</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1111</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G5">
+        <v>17410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>245</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1111</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G6">
+        <v>17410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1111</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G7">
+        <v>17610</v>
       </c>
     </row>
   </sheetData>
@@ -1904,9 +2127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1936,6 +2157,293 @@
       </c>
       <c r="B3" s="20">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" s="22">
+        <v>5210</v>
+      </c>
+      <c r="E2" s="22">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3" s="22">
+        <v>5211</v>
+      </c>
+      <c r="E3" s="22">
+        <v>0</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="17">
+        <v>17410</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D5" s="17">
+        <v>17610</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="K5" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="L5" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:B5" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="B4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2527,7 +3035,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3008,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
commit pritam test case
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="3024" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="3024" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="294">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -844,6 +844,81 @@
   </si>
   <si>
     <t>31/12/2020</t>
+  </si>
+  <si>
+    <t>Leafnode</t>
+  </si>
+  <si>
+    <t>ASHOK1.1</t>
+  </si>
+  <si>
+    <t>CategoryPosterImage_NL</t>
+  </si>
+  <si>
+    <t>http://10.67.191.50:8085/posterserver/poster/vod/w-210_h-280/tf1_0000000001854134.jpg</t>
+  </si>
+  <si>
+    <t>CategoryPosterImage_FL</t>
+  </si>
+  <si>
+    <t>http://10.67.191.50:8085/posterserver/poster/vod/w-210_h-280/sky_902662710999frm23.jpg</t>
+  </si>
+  <si>
+    <t>RecentPoster_NL</t>
+  </si>
+  <si>
+    <t>13days.jpg</t>
+  </si>
+  <si>
+    <t>DeafultPoster_FR</t>
+  </si>
+  <si>
+    <t>Default_poster_FR</t>
+  </si>
+  <si>
+    <t>Poster_Navigation_NL</t>
+  </si>
+  <si>
+    <t>Preview KIDS</t>
+  </si>
+  <si>
+    <t>Poster_Navigation_FR</t>
+  </si>
+  <si>
+    <t>Puneet1Euro2</t>
+  </si>
+  <si>
+    <t>Navigate_NL_Leaf</t>
+  </si>
+  <si>
+    <t>commedesrois.jpg</t>
+  </si>
+  <si>
+    <t>Navigate_FR_Leaf</t>
+  </si>
+  <si>
+    <t>sky_902662710999frm23.jpg</t>
+  </si>
+  <si>
+    <t>Navigate_NL_NonLeaf</t>
+  </si>
+  <si>
+    <t>ASHOK1NL</t>
+  </si>
+  <si>
+    <t>DeafultPoster_NL</t>
+  </si>
+  <si>
+    <t>Default_poster_NL</t>
+  </si>
+  <si>
+    <t>Navigate_New_Poster_NL</t>
+  </si>
+  <si>
+    <t>sky_904078115401nlm02.jpg</t>
+  </si>
+  <si>
+    <t>Navigate_New_Poster_FR</t>
   </si>
 </sst>
 </file>
@@ -853,7 +928,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -896,6 +971,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -924,7 +1006,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -988,6 +1070,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1569,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -3032,10 +3115,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3215,6 +3298,14 @@
       </c>
       <c r="B20" s="20" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -3283,16 +3374,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -3335,7 +3426,106 @@
         <v>205</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>286</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3516,7 +3706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update xpath in EPG and Release dopdown contain current execution result value
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Automation\HTML\HTMLSelenium\src\test\java\com\rsystems\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="3024" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4032" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -32,7 +27,8 @@
     <sheet name="PackageAssignAndUnassign" sheetId="22" r:id="rId18"/>
     <sheet name="MovieScreen" sheetId="23" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0" calcMode="manual"/>
+  <oleSize ref="A8:D19"/>
 </workbook>
 </file>
 
@@ -1652,7 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -2210,7 +2206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2239,7 +2237,7 @@
         <v>214</v>
       </c>
       <c r="B3" s="20">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3706,8 +3704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3845,7 +3843,7 @@
         <v>228</v>
       </c>
       <c r="B16" s="20">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3853,7 +3851,7 @@
         <v>229</v>
       </c>
       <c r="B17" s="20">
-        <v>47</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rahul test case mini EPG and STB assign and Unassign using API
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Perforce\faheem.khan_c1-gf-102_4562\bgc\Automation\HTML\HTMLSelenium\src\test\java\com\rsystems\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4032" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4032" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -28,12 +33,11 @@
     <sheet name="MovieScreen" sheetId="23" r:id="rId19"/>
   </sheets>
   <calcPr calcId="0" calcMode="manual"/>
-  <oleSize ref="A8:D19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="302">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -915,6 +919,30 @@
   </si>
   <si>
     <t>Navigate_New_Poster_FR</t>
+  </si>
+  <si>
+    <t>Pause Live TV</t>
+  </si>
+  <si>
+    <t>Pause Live TV Free</t>
+  </si>
+  <si>
+    <t>PLTV</t>
+  </si>
+  <si>
+    <t>PLTVFREE</t>
+  </si>
+  <si>
+    <t>EquipmentId</t>
+  </si>
+  <si>
+    <t>MacAddress</t>
+  </si>
+  <si>
+    <t>SubscriberVersion</t>
+  </si>
+  <si>
+    <t>2CABA452DEF1</t>
   </si>
 </sst>
 </file>
@@ -1943,15 +1971,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1985,6 +2013,38 @@
       </c>
       <c r="B4" s="17" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1854816</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="17">
+        <v>254479921</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2247,10 +2307,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2437,10 +2497,76 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="17">
+        <v>173</v>
+      </c>
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>268</v>
+      </c>
       <c r="K6" t="s">
         <v>54</v>
       </c>
       <c r="L6" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="17">
+        <v>231</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>240</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="24" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2448,7 +2574,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B2:B5" numberStoredAsText="1"/>
+    <ignoredError sqref="B2:B7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3704,7 +3830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
commit pritam test cases and all test case xml
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4032" firstSheet="7" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4032" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="308">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -943,6 +943,24 @@
   </si>
   <si>
     <t>2CABA452DEF1</t>
+  </si>
+  <si>
+    <t>CUTVDisabledChannel_1</t>
+  </si>
+  <si>
+    <t>CUTVDisabledChannel_2</t>
+  </si>
+  <si>
+    <t>CUTVDisabledChannel_3</t>
+  </si>
+  <si>
+    <t>CUTVDisabledChannel_4</t>
+  </si>
+  <si>
+    <t>CUTVDisabledChannel_5</t>
+  </si>
+  <si>
+    <t>CUTVDisabledChannel_6</t>
   </si>
 </sst>
 </file>
@@ -1973,7 +1991,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3828,10 +3846,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3980,6 +3998,54 @@
         <v>3</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B18" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B19" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B20" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="B22" s="20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B23" s="20">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" display="http://hpg.nat.myrio.net:8080/bepweb-1.0/resources/common/images/Play_ON.png"/>

</xml_diff>

<commit_message>
Create new test casesclear
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="4032" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4968" firstSheet="14" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -31,13 +31,14 @@
     <sheet name="Recording" sheetId="21" r:id="rId17"/>
     <sheet name="PackageAssignAndUnassign" sheetId="22" r:id="rId18"/>
     <sheet name="MovieScreen" sheetId="23" r:id="rId19"/>
+    <sheet name="SettingScreen" sheetId="24" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="0" calcMode="manual"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="320">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -961,6 +962,42 @@
   </si>
   <si>
     <t>CUTVDisabledChannel_6</t>
+  </si>
+  <si>
+    <t>Option1</t>
+  </si>
+  <si>
+    <t>Option2</t>
+  </si>
+  <si>
+    <t>Option3</t>
+  </si>
+  <si>
+    <t>Option4</t>
+  </si>
+  <si>
+    <t>Option5</t>
+  </si>
+  <si>
+    <t>Option6</t>
+  </si>
+  <si>
+    <t>Option7</t>
+  </si>
+  <si>
+    <t>mijn account</t>
+  </si>
+  <si>
+    <t>kinderslot</t>
+  </si>
+  <si>
+    <t>aanbevelingen</t>
+  </si>
+  <si>
+    <t>zenders hernummeren</t>
+  </si>
+  <si>
+    <t>beheer van de toestellen</t>
   </si>
 </sst>
 </file>
@@ -2109,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2272,6 +2309,11 @@
       </c>
       <c r="G7">
         <v>17610</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2599,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2613,7 +2655,7 @@
     <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2627,7 +2669,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>259</v>
       </c>
@@ -2638,7 +2680,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>260</v>
       </c>
@@ -2649,7 +2691,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>261</v>
       </c>
@@ -2660,7 +2702,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>262</v>
       </c>
@@ -2669,6 +2711,11 @@
       </c>
       <c r="C5" s="20" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -3078,6 +3125,90 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
@@ -3848,7 +3979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add some test cases route console log to file
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4968" firstSheet="14" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4968" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="321">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -998,6 +998,9 @@
   </si>
   <si>
     <t>beheer van de toestellen</t>
+  </si>
+  <si>
+    <t>search</t>
   </si>
 </sst>
 </file>
@@ -3129,7 +3132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -3388,10 +3391,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3579,6 +3582,14 @@
       </c>
       <c r="B21" s="20" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" t="s">
+        <v>320</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Testdata and create new DTVTest.xml
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4968" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4968" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -3393,7 +3393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3990,8 +3990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4081,7 +4081,7 @@
         <v>210</v>
       </c>
       <c r="B10" s="20">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
STB update account information
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit.agarwal1\Perforce\faheem.khan_c1-gf-102_4562\bgc\Automation\HTML\HTMLSelenium\src\test\java\com\rsystems\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="4968" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17124" windowHeight="3780" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -34,6 +29,7 @@
     <sheet name="SettingScreen" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:O11"/>
 </workbook>
 </file>
 
@@ -943,9 +939,6 @@
     <t>SubscriberVersion</t>
   </si>
   <si>
-    <t>2CABA452DEF1</t>
-  </si>
-  <si>
     <t>CUTVDisabledChannel_1</t>
   </si>
   <si>
@@ -1001,6 +994,9 @@
   </si>
   <si>
     <t>search</t>
+  </si>
+  <si>
+    <t>2CABA452DED5</t>
   </si>
 </sst>
 </file>
@@ -2031,8 +2027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2078,7 +2074,7 @@
         <v>298</v>
       </c>
       <c r="B5" s="17">
-        <v>1854816</v>
+        <v>1849018</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2086,7 +2082,7 @@
         <v>299</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2094,7 +2090,7 @@
         <v>94</v>
       </c>
       <c r="B7" s="17">
-        <v>254479921</v>
+        <v>254479723</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3152,31 +3148,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>31</v>
@@ -3184,15 +3180,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>103</v>
@@ -3200,10 +3196,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -3589,7 +3585,7 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3990,7 +3986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -4142,7 +4138,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B18" s="20">
         <v>1</v>
@@ -4150,7 +4146,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B19" s="20">
         <v>2</v>
@@ -4158,7 +4154,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B20" s="20">
         <v>4</v>
@@ -4166,7 +4162,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B21" s="20">
         <v>6</v>
@@ -4174,7 +4170,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B22" s="20">
         <v>7</v>
@@ -4182,7 +4178,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B23" s="20">
         <v>9</v>

</xml_diff>

<commit_message>
commit test cases for Sprint 5
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul.Dhoundiyal\Documents\Work\18-08-2017\HTMLSelenium\src\test\java\com\rsystems\config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17124" windowHeight="3780" firstSheet="13" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17130" windowHeight="3780" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -29,12 +34,11 @@
     <sheet name="SettingScreen" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="322">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -997,6 +1001,9 @@
   </si>
   <si>
     <t>2CABA452DED5</t>
+  </si>
+  <si>
+    <t>ChannelWithLeastDurationEpisode</t>
   </si>
 </sst>
 </file>
@@ -1460,24 +1467,24 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.44140625" customWidth="1"/>
-    <col min="7" max="9" width="12.109375" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1"/>
-    <col min="13" max="13" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" customWidth="1"/>
     <col min="14" max="14" width="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.88671875" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1524,7 +1531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1556,7 +1563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1588,7 +1595,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1620,7 +1627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1661,7 +1668,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1702,7 +1709,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1734,12 +1741,12 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1747,7 +1754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -1755,7 +1762,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -1763,7 +1770,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1771,7 +1778,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -1779,7 +1786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>213</v>
       </c>
@@ -1787,7 +1794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>215</v>
       </c>
@@ -1795,7 +1802,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>217</v>
       </c>
@@ -1813,16 +1820,16 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1830,7 +1837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>163</v>
       </c>
@@ -1838,7 +1845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>162</v>
       </c>
@@ -1846,7 +1853,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>160</v>
       </c>
@@ -1854,7 +1861,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>158</v>
       </c>
@@ -1862,7 +1869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>157</v>
       </c>
@@ -1870,7 +1877,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>156</v>
       </c>
@@ -1895,13 +1902,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1909,7 +1916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>184</v>
       </c>
@@ -1917,7 +1924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>183</v>
       </c>
@@ -1925,7 +1932,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>181</v>
       </c>
@@ -1933,7 +1940,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>179</v>
       </c>
@@ -1941,7 +1948,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>177</v>
       </c>
@@ -1949,7 +1956,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>175</v>
       </c>
@@ -1957,7 +1964,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>173</v>
       </c>
@@ -1965,7 +1972,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1973,7 +1980,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>170</v>
       </c>
@@ -1995,13 +2002,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2009,7 +2016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -2027,17 +2034,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2045,7 +2052,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -2053,7 +2060,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2061,7 +2068,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2069,7 +2076,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>298</v>
       </c>
@@ -2077,7 +2084,7 @@
         <v>1849018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>299</v>
       </c>
@@ -2085,7 +2092,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -2093,7 +2100,7 @@
         <v>254479723</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>300</v>
       </c>
@@ -2116,13 +2123,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2130,7 +2137,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -2151,17 +2158,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2184,7 +2191,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -2221,7 +2228,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -2241,7 +2248,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -2264,7 +2271,7 @@
         <v>17410</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>245</v>
       </c>
@@ -2287,7 +2294,7 @@
         <v>17410</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -2310,7 +2317,7 @@
         <v>17610</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -2329,13 +2336,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2343,7 +2350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>203</v>
       </c>
@@ -2351,7 +2358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>214</v>
       </c>
@@ -2372,21 +2379,21 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="20" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2415,7 +2422,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>242</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>243</v>
       </c>
@@ -2485,7 +2492,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>247</v>
       </c>
@@ -2520,7 +2527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>248</v>
       </c>
@@ -2555,7 +2562,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>294</v>
       </c>
@@ -2590,7 +2597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>295</v>
       </c>
@@ -2619,12 +2626,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
         <v>54</v>
       </c>
@@ -2646,15 +2653,15 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2668,7 +2675,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>259</v>
       </c>
@@ -2679,7 +2686,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>260</v>
       </c>
@@ -2690,7 +2697,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>261</v>
       </c>
@@ -2701,7 +2708,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>262</v>
       </c>
@@ -2712,7 +2719,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>54</v>
       </c>
@@ -2727,28 +2734,28 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="12.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="9.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="12.88671875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.109375" customWidth="1"/>
-    <col min="15" max="15" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2801,7 +2808,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -2824,7 +2831,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2847,7 +2854,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2870,7 +2877,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2893,7 +2900,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2916,7 +2923,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -2939,7 +2946,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2962,7 +2969,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2985,7 +2992,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -3008,7 +3015,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3031,7 +3038,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3054,7 +3061,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -3077,7 +3084,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3100,7 +3107,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -3108,12 +3115,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M18" s="3" t="s">
         <v>54</v>
       </c>
@@ -3132,13 +3139,13 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3146,7 +3153,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -3154,7 +3161,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>308</v>
       </c>
@@ -3162,7 +3169,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>309</v>
       </c>
@@ -3170,7 +3177,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>310</v>
       </c>
@@ -3178,7 +3185,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>311</v>
       </c>
@@ -3186,7 +3193,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>312</v>
       </c>
@@ -3194,7 +3201,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>313</v>
       </c>
@@ -3216,14 +3223,14 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3240,7 +3247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -3254,7 +3261,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -3268,7 +3275,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -3282,7 +3289,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -3296,7 +3303,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -3310,7 +3317,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -3324,7 +3331,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3338,7 +3345,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3352,7 +3359,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -3366,7 +3373,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3393,14 +3400,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3411,7 +3418,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -3422,7 +3429,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3433,7 +3440,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3444,7 +3451,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -3452,7 +3459,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -3460,7 +3467,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3468,7 +3475,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -3476,7 +3483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -3484,7 +3491,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -3492,7 +3499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>102</v>
       </c>
@@ -3500,7 +3507,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>104</v>
       </c>
@@ -3508,7 +3515,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>106</v>
       </c>
@@ -3516,7 +3523,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>136</v>
       </c>
@@ -3524,7 +3531,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -3532,7 +3539,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>166</v>
       </c>
@@ -3540,7 +3547,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>167</v>
       </c>
@@ -3548,7 +3555,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>221</v>
       </c>
@@ -3556,7 +3563,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>222</v>
       </c>
@@ -3564,7 +3571,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>223</v>
       </c>
@@ -3572,7 +3579,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>269</v>
       </c>
@@ -3580,7 +3587,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
@@ -3601,13 +3608,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3615,7 +3622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -3623,7 +3630,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -3631,7 +3638,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -3639,7 +3646,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -3660,13 +3667,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3674,7 +3681,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -3682,7 +3689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -3690,7 +3697,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3698,7 +3705,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -3706,7 +3713,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>271</v>
       </c>
@@ -3714,7 +3721,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>273</v>
       </c>
@@ -3722,7 +3729,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>275</v>
       </c>
@@ -3730,7 +3737,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>277</v>
       </c>
@@ -3738,7 +3745,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>279</v>
       </c>
@@ -3746,7 +3753,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>281</v>
       </c>
@@ -3754,7 +3761,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>283</v>
       </c>
@@ -3762,7 +3769,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>285</v>
       </c>
@@ -3770,7 +3777,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>287</v>
       </c>
@@ -3778,7 +3785,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>289</v>
       </c>
@@ -3786,7 +3793,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>291</v>
       </c>
@@ -3794,7 +3801,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>293</v>
       </c>
@@ -3818,14 +3825,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5546875" customWidth="1"/>
-    <col min="2" max="2" width="33.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3833,7 +3840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>123</v>
       </c>
@@ -3841,7 +3848,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>134</v>
       </c>
@@ -3849,7 +3856,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>120</v>
       </c>
@@ -3857,7 +3864,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>119</v>
       </c>
@@ -3865,7 +3872,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>117</v>
       </c>
@@ -3873,7 +3880,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>115</v>
       </c>
@@ -3881,7 +3888,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>113</v>
       </c>
@@ -3889,7 +3896,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>111</v>
       </c>
@@ -3897,7 +3904,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>110</v>
       </c>
@@ -3905,7 +3912,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>108</v>
       </c>
@@ -3913,15 +3920,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
@@ -3939,12 +3946,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3955,7 +3962,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -3966,7 +3973,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -3984,20 +3991,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -4005,7 +4012,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -4013,7 +4020,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -4021,7 +4028,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -4029,7 +4036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -4037,7 +4044,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -4045,7 +4052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -4053,7 +4060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -4064,7 +4071,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -4072,15 +4079,15 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>210</v>
       </c>
       <c r="B10" s="20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>211</v>
       </c>
@@ -4088,7 +4095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>224</v>
       </c>
@@ -4096,47 +4103,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>225</v>
       </c>
       <c r="B13" s="20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>226</v>
       </c>
       <c r="B14" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>227</v>
       </c>
       <c r="B15" s="20">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>228</v>
       </c>
       <c r="B16" s="20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>229</v>
       </c>
       <c r="B17" s="20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>301</v>
       </c>
@@ -4144,7 +4151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>302</v>
       </c>
@@ -4152,7 +4159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>303</v>
       </c>
@@ -4160,7 +4167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>304</v>
       </c>
@@ -4168,7 +4175,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
         <v>305</v>
       </c>
@@ -4176,12 +4183,20 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>306</v>
       </c>
       <c r="B23" s="20">
         <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update PVR channel number
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul.Dhoundiyal\Documents\Work\18-08-2017\HTMLSelenium\src\test\java\com\rsystems\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17130" windowHeight="3780" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="13" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -34,6 +29,7 @@
     <sheet name="SettingScreen" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:N12"/>
 </workbook>
 </file>
 
@@ -1467,24 +1463,24 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" customWidth="1"/>
     <col min="14" max="14" width="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="15" max="15" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1531,7 +1527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1563,7 +1559,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1595,7 +1591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1627,7 +1623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1668,7 +1664,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1705,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1741,12 +1737,12 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1754,7 +1750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>153</v>
       </c>
@@ -1762,7 +1758,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -1770,7 +1766,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1778,7 +1774,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -1786,7 +1782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>213</v>
       </c>
@@ -1794,7 +1790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>215</v>
       </c>
@@ -1802,7 +1798,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>217</v>
       </c>
@@ -1823,13 +1819,13 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1837,7 +1833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>163</v>
       </c>
@@ -1845,7 +1841,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>162</v>
       </c>
@@ -1853,7 +1849,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>160</v>
       </c>
@@ -1861,7 +1857,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>158</v>
       </c>
@@ -1869,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>157</v>
       </c>
@@ -1877,7 +1873,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>156</v>
       </c>
@@ -1902,13 +1898,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -1916,7 +1912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>184</v>
       </c>
@@ -1924,7 +1920,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>183</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>181</v>
       </c>
@@ -1940,7 +1936,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>179</v>
       </c>
@@ -1948,7 +1944,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>177</v>
       </c>
@@ -1956,7 +1952,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>175</v>
       </c>
@@ -1964,7 +1960,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>173</v>
       </c>
@@ -1972,7 +1968,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>9</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>170</v>
       </c>
@@ -2002,13 +1998,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2016,7 +2012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -2038,13 +2034,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2052,7 +2048,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -2060,7 +2056,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2076,7 +2072,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>298</v>
       </c>
@@ -2084,7 +2080,7 @@
         <v>1849018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>299</v>
       </c>
@@ -2092,7 +2088,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -2100,7 +2096,7 @@
         <v>254479723</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>300</v>
       </c>
@@ -2123,13 +2119,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2137,7 +2133,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -2158,17 +2154,17 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2191,7 +2187,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>196</v>
       </c>
@@ -2208,7 +2204,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>206</v>
       </c>
@@ -2228,7 +2224,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -2248,7 +2244,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>244</v>
       </c>
@@ -2271,7 +2267,7 @@
         <v>17410</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>245</v>
       </c>
@@ -2294,7 +2290,7 @@
         <v>17410</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -2317,7 +2313,7 @@
         <v>17610</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -2332,17 +2328,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2350,7 +2346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>203</v>
       </c>
@@ -2358,12 +2354,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>214</v>
       </c>
       <c r="B3" s="20">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2379,21 +2375,21 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2422,7 +2418,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>242</v>
       </c>
@@ -2457,7 +2453,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>243</v>
       </c>
@@ -2492,7 +2488,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>247</v>
       </c>
@@ -2527,7 +2523,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>248</v>
       </c>
@@ -2562,7 +2558,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>294</v>
       </c>
@@ -2597,7 +2593,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>295</v>
       </c>
@@ -2626,12 +2622,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
         <v>54</v>
       </c>
@@ -2653,15 +2649,15 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2675,7 +2671,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>259</v>
       </c>
@@ -2686,7 +2682,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>260</v>
       </c>
@@ -2697,7 +2693,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>261</v>
       </c>
@@ -2708,7 +2704,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>262</v>
       </c>
@@ -2719,7 +2715,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>54</v>
       </c>
@@ -2737,25 +2733,25 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="12.140625" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.140625" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="12.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.109375" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="12.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.109375" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2808,7 +2804,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -2831,7 +2827,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -2854,7 +2850,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -2877,7 +2873,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -2900,7 +2896,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -2923,7 +2919,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -2946,7 +2942,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -2969,7 +2965,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2992,7 +2988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -3015,7 +3011,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3038,7 +3034,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3061,7 +3057,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -3084,7 +3080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3107,7 +3103,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -3115,12 +3111,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="M18" s="3" t="s">
         <v>54</v>
       </c>
@@ -3139,13 +3135,13 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3153,7 +3149,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>307</v>
       </c>
@@ -3161,7 +3157,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>308</v>
       </c>
@@ -3169,7 +3165,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>309</v>
       </c>
@@ -3177,7 +3173,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>310</v>
       </c>
@@ -3185,7 +3181,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>311</v>
       </c>
@@ -3193,7 +3189,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>312</v>
       </c>
@@ -3201,7 +3197,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>313</v>
       </c>
@@ -3223,14 +3219,14 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3247,7 +3243,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -3261,7 +3257,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -3275,7 +3271,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -3289,7 +3285,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -3303,7 +3299,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -3317,7 +3313,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -3331,7 +3327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3345,7 +3341,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3359,7 +3355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -3373,7 +3369,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3400,14 +3396,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3418,7 +3414,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -3429,7 +3425,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3440,7 +3436,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -3451,7 +3447,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -3459,7 +3455,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -3467,7 +3463,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3475,7 +3471,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -3483,7 +3479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -3491,7 +3487,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -3499,7 +3495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>102</v>
       </c>
@@ -3507,7 +3503,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>104</v>
       </c>
@@ -3515,7 +3511,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>106</v>
       </c>
@@ -3523,7 +3519,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>136</v>
       </c>
@@ -3531,7 +3527,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>9</v>
       </c>
@@ -3539,7 +3535,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>166</v>
       </c>
@@ -3547,7 +3543,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>167</v>
       </c>
@@ -3555,7 +3551,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>221</v>
       </c>
@@ -3563,7 +3559,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>222</v>
       </c>
@@ -3571,7 +3567,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>223</v>
       </c>
@@ -3579,7 +3575,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>269</v>
       </c>
@@ -3587,7 +3583,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
@@ -3608,13 +3604,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -3622,7 +3618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -3630,7 +3626,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -3638,7 +3634,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -3646,7 +3642,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -3667,13 +3663,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="78.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3681,7 +3677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -3689,7 +3685,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -3697,7 +3693,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -3705,7 +3701,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -3713,7 +3709,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>271</v>
       </c>
@@ -3721,7 +3717,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>273</v>
       </c>
@@ -3729,7 +3725,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>275</v>
       </c>
@@ -3737,7 +3733,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
         <v>277</v>
       </c>
@@ -3745,7 +3741,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>279</v>
       </c>
@@ -3753,7 +3749,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>281</v>
       </c>
@@ -3761,7 +3757,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>283</v>
       </c>
@@ -3769,7 +3765,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>285</v>
       </c>
@@ -3777,7 +3773,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>287</v>
       </c>
@@ -3785,7 +3781,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>289</v>
       </c>
@@ -3793,7 +3789,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>291</v>
       </c>
@@ -3801,7 +3797,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>293</v>
       </c>
@@ -3825,14 +3821,14 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.5546875" customWidth="1"/>
+    <col min="2" max="2" width="33.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3840,7 +3836,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>123</v>
       </c>
@@ -3848,7 +3844,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>134</v>
       </c>
@@ -3856,7 +3852,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>120</v>
       </c>
@@ -3864,7 +3860,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>119</v>
       </c>
@@ -3872,7 +3868,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>117</v>
       </c>
@@ -3880,7 +3876,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>115</v>
       </c>
@@ -3888,7 +3884,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>113</v>
       </c>
@@ -3896,7 +3892,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>111</v>
       </c>
@@ -3904,7 +3900,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>110</v>
       </c>
@@ -3912,7 +3908,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>108</v>
       </c>
@@ -3920,15 +3916,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
     </row>
@@ -3946,12 +3942,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3962,7 +3958,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -3973,7 +3969,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -3993,18 +3989,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -4012,7 +4008,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -4020,7 +4016,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>138</v>
       </c>
@@ -4028,7 +4024,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>139</v>
       </c>
@@ -4036,7 +4032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -4044,7 +4040,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -4052,7 +4048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -4060,7 +4056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -4071,7 +4067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>147</v>
       </c>
@@ -4079,7 +4075,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>210</v>
       </c>
@@ -4087,7 +4083,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
         <v>211</v>
       </c>
@@ -4095,7 +4091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>224</v>
       </c>
@@ -4103,7 +4099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>225</v>
       </c>
@@ -4111,7 +4107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
         <v>226</v>
       </c>
@@ -4119,7 +4115,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>227</v>
       </c>
@@ -4127,7 +4123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>228</v>
       </c>
@@ -4135,7 +4131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>229</v>
       </c>
@@ -4143,7 +4139,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
         <v>301</v>
       </c>
@@ -4151,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>302</v>
       </c>
@@ -4159,7 +4155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>303</v>
       </c>
@@ -4167,7 +4163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
         <v>304</v>
       </c>
@@ -4175,7 +4171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
         <v>305</v>
       </c>
@@ -4183,7 +4179,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
         <v>306</v>
       </c>
@@ -4191,7 +4187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>321</v>
       </c>

</xml_diff>

<commit_message>
commit Rahul EPG Test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="355">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -1058,6 +1058,51 @@
   </si>
   <si>
     <t>Opacity</t>
+  </si>
+  <si>
+    <t>top</t>
+  </si>
+  <si>
+    <t>margin-right</t>
+  </si>
+  <si>
+    <t>channelCell</t>
+  </si>
+  <si>
+    <t>64px</t>
+  </si>
+  <si>
+    <t>nonFocussedCell</t>
+  </si>
+  <si>
+    <t>focussedCell</t>
+  </si>
+  <si>
+    <t>channelLogo</t>
+  </si>
+  <si>
+    <t>80px</t>
+  </si>
+  <si>
+    <t>46px</t>
+  </si>
+  <si>
+    <t>6px</t>
+  </si>
+  <si>
+    <t>cutvChannelIcon</t>
+  </si>
+  <si>
+    <t>15px</t>
+  </si>
+  <si>
+    <t>5px</t>
+  </si>
+  <si>
+    <t>epg_channel_number</t>
+  </si>
+  <si>
+    <t>NonFocusCell</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1117,6 +1162,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1141,11 +1193,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1210,10 +1263,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2785,35 +2844,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="8" width="15.33203125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="15.33203125" style="20" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" style="20" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2883,12 +2941,18 @@
       <c r="W1" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="X1" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y1" s="30" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="20" t="s">
         <v>42</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -2897,47 +2961,51 @@
       <c r="S2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="20">
         <v>6</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="20">
         <v>4</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S4" s="3" t="s">
@@ -2946,253 +3014,277 @@
       <c r="U4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="20">
         <v>4</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="20">
         <v>4</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U6" t="s">
+      <c r="U6" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="20">
         <v>4</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="20">
         <v>4</v>
       </c>
-      <c r="W7" t="s">
+      <c r="W7" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="20">
         <v>4</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="20">
         <v>6</v>
       </c>
-      <c r="W9" t="s">
+      <c r="W9" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U10" t="s">
+      <c r="U10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="20">
         <v>6</v>
       </c>
-      <c r="W10" t="s">
+      <c r="W10" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="20">
         <v>6</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R12" t="s">
+      <c r="R12" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U12" t="s">
+      <c r="U12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="20">
         <v>6</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U13" t="s">
+      <c r="U13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="20">
         <v>6</v>
       </c>
-      <c r="W13" t="s">
+      <c r="W13" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="20" t="s">
         <v>43</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U14" t="s">
+      <c r="U14" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="20">
         <v>6</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
         <v>322</v>
       </c>
       <c r="D16" s="20" t="s">
@@ -3204,12 +3296,14 @@
       <c r="R16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="S16" t="s">
+      <c r="S16" s="20" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>325</v>
       </c>
       <c r="C17" s="20" t="s">
@@ -3219,8 +3313,8 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
         <v>326</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -3233,8 +3327,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
         <v>327</v>
       </c>
       <c r="C19" s="20" t="s">
@@ -3244,8 +3338,8 @@
         <v>333</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>328</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -3255,8 +3349,8 @@
         <v>333</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
         <v>334</v>
       </c>
       <c r="F21" s="20">
@@ -3274,16 +3368,92 @@
       <c r="S21" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="U21" t="s">
+      <c r="U21" s="20" t="s">
         <v>16</v>
       </c>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A22" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A23" s="31" t="s">
+        <v>344</v>
+      </c>
+      <c r="H23" s="20">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A24" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="H24" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A25" s="31" t="s">
+        <v>346</v>
+      </c>
+      <c r="N25" s="31" t="s">
+        <v>347</v>
+      </c>
+      <c r="O25" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="X25" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="Y25" s="31" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A26" s="31" t="s">
+        <v>350</v>
+      </c>
+      <c r="N26" s="31" t="s">
+        <v>351</v>
+      </c>
+      <c r="O26" s="31"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="R27" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="S27" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>354</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="X28" s="31"/>
+      <c r="Y28" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C18" twoDigitTextYear="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
commit new test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="10" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="360">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -1115,6 +1115,9 @@
   </si>
   <si>
     <t>NonReplayChannelProgramInPast</t>
+  </si>
+  <si>
+    <t>BlackProgramChannelNumber</t>
   </si>
 </sst>
 </file>
@@ -2465,8 +2468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2867,7 +2870,7 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4354,10 +4357,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4562,6 +4565,11 @@
         <v>47</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>359</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" display="http://hpg.nat.myrio.net:8080/bepweb-1.0/resources/common/images/Play_ON.png"/>

</xml_diff>

<commit_message>
commit for BVt execution
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -2566,8 +2566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2597,7 +2597,7 @@
         <v>214</v>
       </c>
       <c r="B3" s="20">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -3782,7 +3782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commit Testcase sheet file
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -2276,7 +2276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4621,8 +4621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
commit pritam bug fixes
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="9" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="396">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -547,12 +547,6 @@
     <t>op aanvraag</t>
   </si>
   <si>
-    <t>maa 19 jun</t>
-  </si>
-  <si>
-    <t>DateTime</t>
-  </si>
-  <si>
     <t>een tv-programma zoeken</t>
   </si>
   <si>
@@ -1229,14 +1223,18 @@
   </si>
   <si>
     <t>Verkeerde aankooppincode. Probeer opnieuw.</t>
+  </si>
+  <si>
+    <t>WrongPinNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1344,7 +1342,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1421,6 +1419,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2046,7 +2047,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B5" s="17">
         <v>10</v>
@@ -2054,7 +2055,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B6" s="17">
         <v>20</v>
@@ -2062,18 +2063,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2162,10 +2163,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2184,7 +2185,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>10</v>
@@ -2192,50 +2193,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2243,14 +2244,6 @@
         <v>9</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="14" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2284,10 +2277,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2315,20 +2308,20 @@
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B3" s="17">
         <v>1111</v>
@@ -2336,7 +2329,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>121</v>
@@ -2344,7 +2337,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B5" s="17">
         <v>1849018</v>
@@ -2352,10 +2345,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2368,10 +2361,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +2380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2402,23 +2395,23 @@
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -2429,10 +2422,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2441,160 +2434,167 @@
     <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C3" t="s">
         <v>207</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="E3" s="17">
         <v>1111</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="38">
+        <v>2222</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E4" s="17">
         <v>1111</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G4" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E5" s="17">
         <v>1111</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="G5">
+      <c r="G5" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H5">
         <v>17410</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B6" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>249</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E6" s="17">
         <v>1111</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="G6">
+      <c r="G6" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H6">
         <v>17410</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B7" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>250</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="17">
         <v>1111</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="G7">
+      <c r="G7" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7">
         <v>17610</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -2629,7 +2629,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B3" s="20">
         <v>15</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B4" s="20">
         <v>16</v>
@@ -2653,7 +2653,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B5" s="20">
         <v>2</v>
@@ -2691,39 +2691,39 @@
         <v>30</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="D1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="H1" s="26" t="s">
         <v>234</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="I1" s="26" t="s">
         <v>235</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D2" s="22">
         <v>5210</v>
@@ -2732,16 +2732,16 @@
         <v>0</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G2" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>54</v>
@@ -2752,13 +2752,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D3" s="22">
         <v>5211</v>
@@ -2767,16 +2767,16 @@
         <v>0</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K3" s="23" t="s">
         <v>54</v>
@@ -2787,13 +2787,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D4" s="17">
         <v>17410</v>
@@ -2802,16 +2802,16 @@
         <v>0</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K4" s="25" t="s">
         <v>54</v>
@@ -2822,13 +2822,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D5" s="17">
         <v>17610</v>
@@ -2837,16 +2837,16 @@
         <v>0</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K5" s="25" t="s">
         <v>54</v>
@@ -2857,13 +2857,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D6" s="17">
         <v>173</v>
@@ -2872,16 +2872,16 @@
         <v>0</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K6" t="s">
         <v>54</v>
@@ -2892,13 +2892,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D7" s="17">
         <v>231</v>
@@ -2907,16 +2907,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2956,10 +2956,10 @@
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D1" s="21" t="s">
         <v>54</v>
@@ -2967,46 +2967,46 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -3057,25 +3057,25 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>24</v>
@@ -3123,10 +3123,10 @@
         <v>85</v>
       </c>
       <c r="Y1" s="30" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="Z1" s="30" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -3137,7 +3137,7 @@
         <v>42</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>17</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>36</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>73</v>
@@ -3478,31 +3478,31 @@
         <v>43</v>
       </c>
       <c r="T16" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="Y16" s="31"/>
       <c r="Z16" s="31"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C18" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>330</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>332</v>
       </c>
       <c r="T18" s="3" t="s">
         <v>54</v>
@@ -3510,29 +3510,29 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>329</v>
-      </c>
       <c r="E20" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G21" s="20">
         <v>278</v>
@@ -3544,10 +3544,10 @@
         <v>0.7</v>
       </c>
       <c r="S21" s="20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="V21" s="20" t="s">
         <v>16</v>
@@ -3557,15 +3557,15 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I23" s="20">
         <v>0.7</v>
@@ -3573,7 +3573,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I24" s="20">
         <v>0</v>
@@ -3581,50 +3581,50 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
+        <v>343</v>
+      </c>
+      <c r="O25" s="31" t="s">
+        <v>344</v>
+      </c>
+      <c r="P25" s="31" t="s">
         <v>345</v>
       </c>
-      <c r="O25" s="31" t="s">
+      <c r="Y25" s="31" t="s">
         <v>346</v>
       </c>
-      <c r="P25" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="Y25" s="31" t="s">
-        <v>348</v>
-      </c>
       <c r="Z25" s="31" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="O26" s="31" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="P26" s="31"/>
       <c r="Y26" s="31"/>
       <c r="Z26" s="31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="S27" s="31" t="s">
         <v>73</v>
       </c>
       <c r="T27" s="31" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="Y27" s="31"/>
       <c r="Z27" s="31"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="32" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>73</v>
@@ -3634,7 +3634,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="I29" s="34">
         <v>0.4</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F30" s="20">
         <v>40</v>
@@ -3651,10 +3651,10 @@
         <v>227</v>
       </c>
       <c r="O30" s="20" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="P30" s="20" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
@@ -3668,15 +3668,15 @@
         <v>68</v>
       </c>
       <c r="T31" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="S32" s="20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="T32" s="20" t="s">
         <v>17</v>
@@ -3684,10 +3684,10 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="S33" s="20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="T33" s="20" t="s">
         <v>17</v>
@@ -3695,10 +3695,10 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="S34" s="20" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="T34" s="20" t="s">
         <v>17</v>
@@ -3706,56 +3706,56 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="O35" s="20" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="S36" s="20" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="V38" s="20" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I39" s="20">
         <v>0.3</v>
       </c>
       <c r="O39" s="20" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I40" s="20">
         <v>1</v>
       </c>
       <c r="O40" s="20" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3783,36 +3783,36 @@
         <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>31</v>
@@ -3820,15 +3820,15 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>103</v>
@@ -3836,10 +3836,10 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>150</v>
@@ -4198,7 +4198,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>152</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>148</v>
@@ -4214,10 +4214,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -4225,7 +4225,7 @@
         <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -4340,106 +4340,106 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -4555,74 +4555,74 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B14" s="35" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -4774,7 +4774,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B10" s="20">
         <v>16</v>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B11" s="20">
         <v>1</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B12" s="20">
         <v>5</v>
@@ -4798,7 +4798,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B13" s="20">
         <v>16</v>
@@ -4806,7 +4806,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B14" s="20">
         <v>30</v>
@@ -4814,7 +4814,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B15" s="20">
         <v>33</v>
@@ -4822,7 +4822,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B16" s="20">
         <v>34</v>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B17" s="20">
         <v>35</v>
@@ -4838,7 +4838,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B18" s="20">
         <v>1</v>
@@ -4846,7 +4846,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B19" s="20">
         <v>2</v>
@@ -4854,7 +4854,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B20" s="20">
         <v>4</v>
@@ -4862,7 +4862,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B21" s="20">
         <v>6</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B22" s="20">
         <v>7</v>
@@ -4878,7 +4878,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B23" s="20">
         <v>9</v>
@@ -4886,7 +4886,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B24">
         <v>47</v>

</xml_diff>

<commit_message>
commit new developed test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -2296,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4689,7 +4689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fixes of EPG changes
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="398">
   <si>
     <t>mijn biblotheek</t>
   </si>
@@ -1099,9 +1099,6 @@
     <t>DayInFrench</t>
   </si>
   <si>
-    <t>maintenant</t>
-  </si>
-  <si>
     <t>DayInDutch</t>
   </si>
   <si>
@@ -1229,6 +1226,12 @@
   </si>
   <si>
     <t>RadioChannel_1</t>
+  </si>
+  <si>
+    <t>aujourd'hui</t>
+  </si>
+  <si>
+    <t>vandaag</t>
   </si>
 </sst>
 </file>
@@ -2411,10 +2414,10 @@
     </row>
     <row r="3" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>393</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -2427,7 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -2459,7 +2462,7 @@
         <v>205</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>251</v>
@@ -2648,7 +2651,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B4" s="20">
         <v>16</v>
@@ -2656,7 +2659,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B5" s="20">
         <v>2</v>
@@ -2770,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>238</v>
@@ -3063,7 +3066,7 @@
         <v>326</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>329</v>
@@ -3637,7 +3640,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I29" s="34">
         <v>0.4</v>
@@ -3645,7 +3648,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F30" s="20">
         <v>40</v>
@@ -3654,10 +3657,10 @@
         <v>227</v>
       </c>
       <c r="O30" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="P30" s="20" t="s">
         <v>365</v>
-      </c>
-      <c r="P30" s="20" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.3">
@@ -3676,10 +3679,10 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S32" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="T32" s="20" t="s">
         <v>17</v>
@@ -3687,10 +3690,10 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S33" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="T33" s="20" t="s">
         <v>17</v>
@@ -3698,10 +3701,10 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S34" s="20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="T34" s="20" t="s">
         <v>17</v>
@@ -3709,56 +3712,56 @@
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O35" s="20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S36" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
+        <v>386</v>
+      </c>
+      <c r="V38" s="20" t="s">
         <v>387</v>
-      </c>
-      <c r="V38" s="20" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I39" s="20">
         <v>0.3</v>
       </c>
       <c r="O39" s="20" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I40" s="20">
         <v>1</v>
       </c>
       <c r="O40" s="20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -4457,8 +4460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4561,71 +4564,71 @@
         <v>352</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>353</v>
+        <v>396</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>178</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B14" s="35" t="s">
         <v>370</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>372</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B16" s="35" t="s">
         <v>374</v>
-      </c>
-      <c r="B16" s="35" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B17" s="36" t="s">
         <v>376</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B18" s="35" t="s">
         <v>378</v>
-      </c>
-      <c r="B18" s="35" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="B19" s="35" t="s">
         <v>380</v>
-      </c>
-      <c r="B19" s="35" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>382</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -4905,7 +4908,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B26" s="20">
         <v>801</v>

</xml_diff>

<commit_message>
change recording channel number
</commit_message>
<xml_diff>
--- a/src/test/java/com/rsystems/config/testdata.xlsx
+++ b/src/test/java/com/rsystems/config/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4056" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="hub" sheetId="2" r:id="rId1"/>
@@ -2615,7 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2646,7 +2646,7 @@
         <v>212</v>
       </c>
       <c r="B3" s="20">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4460,7 +4460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>